<commit_message>
completed dGLN3 input sheet
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/14-genes_35-edges_BK-dGLN3-fam_no-strains-added_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/14-genes_35-edges_BK-dGLN3-fam_no-strains-added_Sigmoid_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="0" windowWidth="25120" windowHeight="14980" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="39">
   <si>
     <t>CIN5</t>
   </si>
@@ -138,13 +138,19 @@
   <si>
     <t>dgln3</t>
   </si>
+  <si>
+    <t>optimization_parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -203,7 +209,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,17 +327,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -390,6 +400,7 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,50 +459,10 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1945,7 +1916,7 @@
       <c r="E4" s="1">
         <v>-6.1600000000000002E-2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.36909999999999998</v>
       </c>
       <c r="G4" s="1">
@@ -2147,7 +2118,7 @@
       <c r="D9" s="1">
         <v>1.8004</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>1.1870000000000001</v>
       </c>
       <c r="F9" s="1">
@@ -2285,7 +2256,7 @@
       <c r="I12" s="1">
         <v>-0.4289</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>-0.10260000000000001</v>
       </c>
       <c r="K12" s="1">
@@ -2335,7 +2306,7 @@
       <c r="L13" s="1">
         <v>-2.0569000000000002</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <v>-1.0194000000000001</v>
       </c>
     </row>
@@ -2384,7 +2355,7 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.45540000000000003</v>
       </c>
       <c r="C15" s="1">
@@ -3891,10 +3862,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B10" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3905,171 +3876,180 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3">
-        <v>2E-3</v>
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3">
-        <v>100000000</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9.9999999999999995E-7</v>
+        <v>20</v>
+      </c>
+      <c r="B4" s="7">
+        <v>100000000</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3">
-        <v>100000000</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="7">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3">
-        <v>9.9999999999999995E-7</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="7">
+        <v>100000000</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="7">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="5">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="5">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1">
         <v>30</v>
       </c>
-      <c r="D13" s="1">
-        <v>60</v>
+      <c r="B13" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="B14" s="4">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <v>10</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>15</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <v>20</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G16" s="1">
         <v>25</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H16" s="1">
         <v>30</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I16" s="1">
         <v>35</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J16" s="1">
         <v>40</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K16" s="1">
         <v>45</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L16" s="1">
         <v>50</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M16" s="1">
         <v>55</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N16" s="1">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated production & degradation rates
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/14-genes_35-edges_BK-dGLN3-fam_no-strains-added_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/14-genes_35-edges_BK-dGLN3-fam_no-strains-added_Sigmoid_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="13380" yWindow="0" windowWidth="18760" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="7" r:id="rId1"/>
@@ -209,7 +209,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -329,8 +329,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,8 +350,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -401,6 +412,11 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -460,6 +476,11 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -791,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -815,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.2009122262492595</v>
+        <v>-0.2009</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -823,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.30806541358219791</v>
+        <v>-0.30809999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -831,7 +852,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.19254088348887369</v>
+        <v>-0.1925</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -839,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.32239403746974199</v>
+        <v>-0.32240000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -847,15 +868,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>-0.27182242374899818</v>
+        <v>-0.27179999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>-9.9021025794277892E-2</v>
+      <c r="B7" s="9">
+        <v>-9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -863,7 +884,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.40773363562349724</v>
+        <v>-0.40770000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -871,7 +892,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.2772588722239781</v>
+        <v>-0.27729999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -879,7 +900,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.69314718055994529</v>
+        <v>-0.69310000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -887,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>-0.28291721655507968</v>
+        <v>-0.28289999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -895,7 +916,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>-0.32239403746974199</v>
+        <v>-0.32240000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -903,7 +924,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.55451774444795621</v>
+        <v>-0.55449999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -911,7 +932,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>-0.17328679513998632</v>
+        <v>-0.17330000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -919,7 +940,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.72962861111573196</v>
+        <v>-0.72960000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +959,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -961,15 +982,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.10045611312462975</v>
+        <v>-0.10050000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>-0.15403270679109896</v>
+      <c r="B3" s="9">
+        <v>-0.154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -977,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>-9.6270441744436844E-2</v>
+        <v>-9.6299999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -985,7 +1006,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.16119701873487099</v>
+        <v>-0.16120000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -993,7 +1014,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>-0.13591121187449909</v>
+        <v>-0.13589999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1001,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>-4.9510512897138946E-2</v>
+        <v>-4.9500000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1009,7 +1030,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.20386681781174862</v>
+        <v>-0.2039</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1017,7 +1038,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.13862943611198905</v>
+        <v>-0.1386</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1025,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.34657359027997264</v>
+        <v>-0.34660000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1033,7 +1054,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>-0.14145860827753984</v>
+        <v>-0.14149999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1041,7 +1062,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>-0.16119701873487099</v>
+        <v>-0.16120000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1049,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.2772588722239781</v>
+        <v>-0.27729999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1057,7 +1078,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>-8.6643397569993161E-2</v>
+        <v>-8.6599999999999996E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1065,7 +1086,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.36481430555786598</v>
+        <v>-0.36480000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3864,7 +3885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>